<commit_message>
Added exception handling for choice list not appearing in corresponding choices worksheet.
</commit_message>
<xml_diff>
--- a/test/HQ.xlsx
+++ b/test/HQ.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6331" uniqueCount="2375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6331" uniqueCount="2374">
   <si>
     <t>type</t>
   </si>
@@ -5990,6 +5990,9 @@
     <t>level3_list</t>
   </si>
   <si>
+    <t>EA_list</t>
+  </si>
+  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -7535,25 +7538,19 @@
     <t>level3_list_example5</t>
   </si>
   <si>
-    <t>level4_list</t>
-  </si>
-  <si>
-    <t>level4_list_example1</t>
-  </si>
-  <si>
-    <t>Level 4 Geography</t>
-  </si>
-  <si>
-    <t>level4_list_example2</t>
-  </si>
-  <si>
-    <t>level4_list_example3</t>
-  </si>
-  <si>
-    <t>level4_list_example4</t>
-  </si>
-  <si>
-    <t>level4_list_example5</t>
+    <t>EA_list_example1</t>
+  </si>
+  <si>
+    <t>EA_list_example2</t>
+  </si>
+  <si>
+    <t>EA_list_example3</t>
+  </si>
+  <si>
+    <t>EA_list_example4</t>
+  </si>
+  <si>
+    <t>EA_list_example5</t>
   </si>
 </sst>
 </file>
@@ -8150,7 +8147,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -8311,34 +8308,34 @@
       </c>
       <c r="AO1" s="25"/>
       <c r="AP1" s="25" t="s">
-        <v>2335</v>
+        <v>2336</v>
       </c>
       <c r="AQ1" s="25" t="s">
-        <v>2336</v>
+        <v>2337</v>
       </c>
       <c r="AR1" s="30" t="s">
-        <v>2337</v>
+        <v>2338</v>
       </c>
       <c r="AS1" s="30" t="s">
-        <v>2338</v>
+        <v>2339</v>
       </c>
       <c r="AT1" s="30" t="s">
-        <v>2339</v>
+        <v>2340</v>
       </c>
       <c r="AU1" s="30" t="s">
-        <v>2340</v>
+        <v>2341</v>
       </c>
       <c r="AV1" s="30" t="s">
-        <v>2341</v>
+        <v>2342</v>
       </c>
       <c r="AW1" s="30" t="s">
-        <v>2342</v>
+        <v>2343</v>
       </c>
       <c r="AX1" s="30" t="s">
-        <v>2343</v>
+        <v>2344</v>
       </c>
       <c r="AY1" s="30" t="s">
-        <v>2344</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="2" spans="1:51" ht="13" customHeight="1">
@@ -8596,7 +8593,7 @@
         <v>65</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>2334</v>
+        <v>2335</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>66</v>
@@ -8614,7 +8611,7 @@
         <v>68</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>2333</v>
+        <v>2334</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>65</v>
@@ -8698,7 +8695,7 @@
     </row>
     <row r="12" spans="1:51" ht="13" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>1903</v>
+        <v>1904</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>74</v>
@@ -8710,7 +8707,7 @@
         <v>46</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>1922</v>
+        <v>1923</v>
       </c>
       <c r="Q12" s="7" t="s">
         <v>75</v>
@@ -8739,31 +8736,31 @@
       <c r="AO12" s="25"/>
       <c r="AP12" s="25"/>
       <c r="AQ12" s="25" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
       <c r="AR12" s="31" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
       <c r="AS12" s="31" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
       <c r="AT12" s="31" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
       <c r="AU12" s="31" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
       <c r="AV12" s="31" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
       <c r="AW12" s="31" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
       <c r="AX12" s="31" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
       <c r="AY12" s="31" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="13" spans="1:51" ht="13" customHeight="1">
@@ -8809,31 +8806,31 @@
       <c r="AO13" s="25"/>
       <c r="AP13" s="25"/>
       <c r="AQ13" s="25" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="AR13" s="31" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="AS13" s="31" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="AT13" s="31" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="AU13" s="31" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="AV13" s="31" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="AW13" s="31" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="AX13" s="31" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="AY13" s="31" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="14" spans="1:51" ht="13" customHeight="1">
@@ -8879,31 +8876,31 @@
       <c r="AO14" s="25"/>
       <c r="AP14" s="25"/>
       <c r="AQ14" s="25" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
       <c r="AR14" s="31" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
       <c r="AS14" s="31" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
       <c r="AT14" s="31" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
       <c r="AU14" s="31" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
       <c r="AV14" s="31" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
       <c r="AW14" s="31" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
       <c r="AX14" s="31" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
       <c r="AY14" s="31" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="15" spans="1:51" ht="13" customHeight="1">
@@ -8949,31 +8946,31 @@
       <c r="AO15" s="25"/>
       <c r="AP15" s="25"/>
       <c r="AQ15" s="25" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="AR15" s="31" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="AS15" s="31" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="AT15" s="31" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="AU15" s="31" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="AV15" s="31" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="AW15" s="31" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="AX15" s="31" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="AY15" s="31" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="16" spans="1:51" ht="13" customHeight="1">
@@ -9590,7 +9587,7 @@
         <v>122</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>1901</v>
+        <v>1902</v>
       </c>
       <c r="J25" s="7" t="s">
         <v>118</v>
@@ -9599,28 +9596,28 @@
         <v>46</v>
       </c>
       <c r="Q25" s="13" t="s">
-        <v>1923</v>
+        <v>1924</v>
       </c>
       <c r="R25" s="13" t="s">
-        <v>2146</v>
+        <v>2147</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>1924</v>
+        <v>1925</v>
       </c>
       <c r="T25" s="13" t="s">
-        <v>1925</v>
+        <v>1926</v>
       </c>
       <c r="U25" s="13" t="s">
-        <v>2291</v>
+        <v>2292</v>
       </c>
       <c r="V25" s="13" t="s">
-        <v>1926</v>
+        <v>1927</v>
       </c>
       <c r="W25" s="13" t="s">
-        <v>1927</v>
+        <v>1928</v>
       </c>
       <c r="X25" s="13" t="s">
-        <v>1928</v>
+        <v>1929</v>
       </c>
       <c r="AO25" s="25"/>
       <c r="AP25" s="25"/>
@@ -9652,7 +9649,7 @@
         <v>124</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>1930</v>
+        <v>1931</v>
       </c>
       <c r="U26" s="7" t="s">
         <v>126</v>
@@ -9678,7 +9675,7 @@
         <v>127</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>2309</v>
+        <v>2310</v>
       </c>
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
@@ -9935,7 +9932,7 @@
         <v>101</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>2329</v>
+        <v>2330</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>144</v>
@@ -9986,7 +9983,7 @@
         <v>148</v>
       </c>
       <c r="AC32" s="18" t="s">
-        <v>2171</v>
+        <v>2172</v>
       </c>
       <c r="AD32" s="18" t="s">
         <v>148</v>
@@ -10169,28 +10166,28 @@
         <v>46</v>
       </c>
       <c r="Q38" s="7" t="s">
-        <v>2252</v>
+        <v>2253</v>
       </c>
       <c r="R38" s="7" t="s">
-        <v>2093</v>
+        <v>2094</v>
       </c>
       <c r="S38" s="7" t="s">
-        <v>2190</v>
+        <v>2191</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="U38" s="7" t="s">
-        <v>2147</v>
+        <v>2148</v>
       </c>
       <c r="V38" s="7" t="s">
-        <v>2253</v>
+        <v>2254</v>
       </c>
       <c r="W38" s="7" t="s">
+        <v>2212</v>
+      </c>
+      <c r="X38" s="7" t="s">
         <v>2211</v>
-      </c>
-      <c r="X38" s="7" t="s">
-        <v>2210</v>
       </c>
       <c r="AO38" s="26"/>
       <c r="AP38" s="26"/>
@@ -10238,22 +10235,22 @@
         <v>46</v>
       </c>
       <c r="Q41" s="7" t="s">
-        <v>2258</v>
+        <v>2259</v>
       </c>
       <c r="R41" s="7" t="s">
-        <v>2094</v>
+        <v>2095</v>
       </c>
       <c r="S41" s="7" t="s">
-        <v>2191</v>
+        <v>2192</v>
       </c>
       <c r="T41" s="7" t="s">
         <v>170</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>2148</v>
+        <v>2149</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>2254</v>
+        <v>2255</v>
       </c>
       <c r="W41" s="7" t="s">
         <v>170</v>
@@ -10291,28 +10288,28 @@
         <v>176</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>2259</v>
+        <v>2260</v>
       </c>
       <c r="R42" s="7" t="s">
-        <v>2095</v>
+        <v>2096</v>
       </c>
       <c r="S42" s="7" t="s">
-        <v>2192</v>
+        <v>2193</v>
       </c>
       <c r="T42" s="7" t="s">
-        <v>1932</v>
+        <v>1933</v>
       </c>
       <c r="U42" s="7" t="s">
-        <v>2149</v>
+        <v>2150</v>
       </c>
       <c r="V42" s="7" t="s">
-        <v>2255</v>
+        <v>2256</v>
       </c>
       <c r="W42" s="7" t="s">
-        <v>2212</v>
+        <v>2213</v>
       </c>
       <c r="X42" s="7" t="s">
-        <v>2213</v>
+        <v>2214</v>
       </c>
       <c r="Y42" s="17" t="s">
         <v>173</v>
@@ -10411,28 +10408,28 @@
         <v>182</v>
       </c>
       <c r="Q45" s="7" t="s">
-        <v>2260</v>
+        <v>2261</v>
       </c>
       <c r="R45" s="7" t="s">
-        <v>2096</v>
+        <v>2097</v>
       </c>
       <c r="S45" s="7" t="s">
-        <v>2193</v>
+        <v>2194</v>
       </c>
       <c r="T45" s="7" t="s">
-        <v>2187</v>
+        <v>2188</v>
       </c>
       <c r="U45" s="7" t="s">
-        <v>2150</v>
+        <v>2151</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>2224</v>
+        <v>2225</v>
       </c>
       <c r="W45" s="7" t="s">
-        <v>2214</v>
+        <v>2215</v>
       </c>
       <c r="X45" s="7" t="s">
-        <v>2215</v>
+        <v>2216</v>
       </c>
       <c r="Y45" s="7" t="s">
         <v>181</v>
@@ -10476,28 +10473,28 @@
         <v>46</v>
       </c>
       <c r="Q46" s="7" t="s">
-        <v>2261</v>
+        <v>2262</v>
       </c>
       <c r="R46" s="7" t="s">
-        <v>2097</v>
+        <v>2098</v>
       </c>
       <c r="S46" s="7" t="s">
-        <v>2194</v>
+        <v>2195</v>
       </c>
       <c r="T46" s="7" t="s">
-        <v>2188</v>
+        <v>2189</v>
       </c>
       <c r="U46" s="7" t="s">
-        <v>2151</v>
+        <v>2152</v>
       </c>
       <c r="V46" s="7" t="s">
-        <v>2256</v>
+        <v>2257</v>
       </c>
       <c r="W46" s="7" t="s">
-        <v>2216</v>
+        <v>2217</v>
       </c>
       <c r="X46" s="7" t="s">
-        <v>2217</v>
+        <v>2218</v>
       </c>
       <c r="AO46" s="25"/>
       <c r="AP46" s="25"/>
@@ -10517,28 +10514,28 @@
         <v>46</v>
       </c>
       <c r="Q47" s="7" t="s">
-        <v>2262</v>
+        <v>2263</v>
       </c>
       <c r="R47" s="7" t="s">
-        <v>2098</v>
+        <v>2099</v>
       </c>
       <c r="S47" s="7" t="s">
-        <v>2195</v>
+        <v>2196</v>
       </c>
       <c r="T47" s="7" t="s">
-        <v>2189</v>
+        <v>2190</v>
       </c>
       <c r="U47" s="7" t="s">
-        <v>2152</v>
+        <v>2153</v>
       </c>
       <c r="V47" s="7" t="s">
-        <v>2257</v>
+        <v>2258</v>
       </c>
       <c r="W47" s="7" t="s">
-        <v>2218</v>
+        <v>2219</v>
       </c>
       <c r="X47" s="7" t="s">
-        <v>2219</v>
+        <v>2220</v>
       </c>
       <c r="AO47" s="26"/>
       <c r="AP47" s="26"/>
@@ -10832,7 +10829,7 @@
         <v>217</v>
       </c>
       <c r="P56" s="7" t="s">
-        <v>2327</v>
+        <v>2328</v>
       </c>
       <c r="AO56" s="28"/>
       <c r="AP56" s="28"/>
@@ -11370,7 +11367,7 @@
         <v>101</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>2330</v>
+        <v>2331</v>
       </c>
       <c r="C76" s="18" t="s">
         <v>277</v>
@@ -11409,7 +11406,7 @@
         <v>277</v>
       </c>
       <c r="Y76" s="18" t="s">
-        <v>2303</v>
+        <v>2304</v>
       </c>
       <c r="Z76" s="18" t="s">
         <v>279</v>
@@ -13308,7 +13305,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>2331</v>
+        <v>2332</v>
       </c>
       <c r="C103" s="18" t="s">
         <v>434</v>
@@ -13589,7 +13586,7 @@
         <v>101</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>2332</v>
+        <v>2333</v>
       </c>
       <c r="C107" s="18" t="s">
         <v>446</v>
@@ -13669,28 +13666,28 @@
         <v>141</v>
       </c>
       <c r="Q108" s="7" t="s">
-        <v>2304</v>
+        <v>2305</v>
       </c>
       <c r="R108" s="7" t="s">
-        <v>2099</v>
+        <v>2100</v>
       </c>
       <c r="S108" s="7" t="s">
-        <v>2225</v>
+        <v>2226</v>
       </c>
       <c r="T108" s="7" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="U108" s="7" t="s">
-        <v>2153</v>
+        <v>2154</v>
       </c>
       <c r="V108" s="7" t="s">
-        <v>2172</v>
+        <v>2173</v>
       </c>
       <c r="W108" s="7" t="s">
-        <v>2220</v>
+        <v>2221</v>
       </c>
       <c r="X108" s="7" t="s">
-        <v>2221</v>
+        <v>2222</v>
       </c>
       <c r="AO108" s="26"/>
       <c r="AP108" s="26"/>
@@ -14048,28 +14045,28 @@
         <v>495</v>
       </c>
       <c r="Q116" s="13" t="s">
-        <v>1935</v>
+        <v>1936</v>
       </c>
       <c r="R116" s="13" t="s">
-        <v>2110</v>
+        <v>2111</v>
       </c>
       <c r="S116" s="13" t="s">
-        <v>1936</v>
+        <v>1937</v>
       </c>
       <c r="T116" s="13" t="s">
-        <v>1937</v>
+        <v>1938</v>
       </c>
       <c r="U116" s="13" t="s">
-        <v>1938</v>
+        <v>1939</v>
       </c>
       <c r="V116" s="13" t="s">
-        <v>1939</v>
+        <v>1940</v>
       </c>
       <c r="W116" s="13" t="s">
-        <v>1940</v>
+        <v>1941</v>
       </c>
       <c r="X116" s="13" t="s">
-        <v>1941</v>
+        <v>1942</v>
       </c>
       <c r="Y116" s="7" t="s">
         <v>492</v>
@@ -14149,28 +14146,28 @@
         <v>498</v>
       </c>
       <c r="Q117" s="13" t="s">
-        <v>1942</v>
+        <v>1943</v>
       </c>
       <c r="R117" s="13" t="s">
-        <v>2111</v>
+        <v>2112</v>
       </c>
       <c r="S117" s="13" t="s">
-        <v>1943</v>
+        <v>1944</v>
       </c>
       <c r="T117" s="13" t="s">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="U117" s="13" t="s">
-        <v>1945</v>
+        <v>1946</v>
       </c>
       <c r="V117" s="13" t="s">
-        <v>1946</v>
+        <v>1947</v>
       </c>
       <c r="W117" s="13" t="s">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="X117" s="13" t="s">
-        <v>1948</v>
+        <v>1949</v>
       </c>
       <c r="Y117" s="7" t="s">
         <v>492</v>
@@ -14302,28 +14299,28 @@
         <v>508</v>
       </c>
       <c r="Q120" s="13" t="s">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="R120" s="13" t="s">
-        <v>2112</v>
+        <v>2113</v>
       </c>
       <c r="S120" s="13" t="s">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="T120" s="13" t="s">
-        <v>1951</v>
+        <v>1952</v>
       </c>
       <c r="U120" s="13" t="s">
-        <v>1952</v>
+        <v>1953</v>
       </c>
       <c r="V120" s="13" t="s">
-        <v>1953</v>
+        <v>1954</v>
       </c>
       <c r="W120" s="13" t="s">
-        <v>1954</v>
+        <v>1955</v>
       </c>
       <c r="X120" s="13" t="s">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="AG120" s="7" t="s">
         <v>476</v>
@@ -14376,28 +14373,28 @@
         <v>508</v>
       </c>
       <c r="Q121" s="7" t="s">
-        <v>2263</v>
+        <v>2264</v>
       </c>
       <c r="R121" s="7" t="s">
-        <v>2113</v>
+        <v>2114</v>
       </c>
       <c r="S121" s="16" t="s">
-        <v>2196</v>
+        <v>2197</v>
       </c>
       <c r="T121" s="7" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="U121" s="7" t="s">
-        <v>2154</v>
+        <v>2155</v>
       </c>
       <c r="V121" s="7" t="s">
-        <v>2173</v>
+        <v>2174</v>
       </c>
       <c r="W121" s="7" t="s">
-        <v>2222</v>
+        <v>2223</v>
       </c>
       <c r="X121" s="7" t="s">
-        <v>2223</v>
+        <v>2224</v>
       </c>
       <c r="Y121" s="7" t="s">
         <v>511</v>
@@ -14447,7 +14444,7 @@
         <v>516</v>
       </c>
       <c r="R122" s="7" t="s">
-        <v>2130</v>
+        <v>2131</v>
       </c>
       <c r="S122" s="7" t="s">
         <v>517</v>
@@ -14494,28 +14491,28 @@
         <v>525</v>
       </c>
       <c r="Q123" s="13" t="s">
-        <v>1956</v>
+        <v>1957</v>
       </c>
       <c r="R123" s="13" t="s">
-        <v>2114</v>
+        <v>2115</v>
       </c>
       <c r="S123" s="13" t="s">
-        <v>1957</v>
+        <v>1958</v>
       </c>
       <c r="T123" s="13" t="s">
-        <v>1958</v>
+        <v>1959</v>
       </c>
       <c r="U123" s="13" t="s">
-        <v>1959</v>
+        <v>1960</v>
       </c>
       <c r="V123" s="13" t="s">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="W123" s="13" t="s">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="X123" s="13" t="s">
-        <v>1962</v>
+        <v>1963</v>
       </c>
       <c r="AG123" s="7" t="s">
         <v>92</v>
@@ -14568,28 +14565,28 @@
         <v>525</v>
       </c>
       <c r="Q124" s="7" t="s">
-        <v>2264</v>
+        <v>2265</v>
       </c>
       <c r="R124" s="7" t="s">
-        <v>2115</v>
+        <v>2116</v>
       </c>
       <c r="S124" s="16" t="s">
-        <v>2197</v>
+        <v>2198</v>
       </c>
       <c r="T124" s="7" t="s">
-        <v>2292</v>
+        <v>2293</v>
       </c>
       <c r="U124" s="7" t="s">
-        <v>2155</v>
+        <v>2156</v>
       </c>
       <c r="V124" s="7" t="s">
-        <v>2174</v>
+        <v>2175</v>
       </c>
       <c r="W124" s="7" t="s">
-        <v>2226</v>
+        <v>2227</v>
       </c>
       <c r="X124" s="7" t="s">
-        <v>2227</v>
+        <v>2228</v>
       </c>
       <c r="Y124" s="7" t="s">
         <v>511</v>
@@ -14639,7 +14636,7 @@
         <v>530</v>
       </c>
       <c r="R125" s="7" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
       <c r="S125" s="7" t="s">
         <v>531</v>
@@ -14648,7 +14645,7 @@
         <v>532</v>
       </c>
       <c r="U125" s="7" t="s">
-        <v>2156</v>
+        <v>2157</v>
       </c>
       <c r="V125" s="7" t="s">
         <v>533</v>
@@ -14689,10 +14686,10 @@
         <v>525</v>
       </c>
       <c r="Q126" s="7" t="s">
-        <v>2312</v>
+        <v>2313</v>
       </c>
       <c r="R126" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S126" s="7" t="s">
         <v>540</v>
@@ -14707,7 +14704,7 @@
         <v>543</v>
       </c>
       <c r="W126" s="7" t="s">
-        <v>2307</v>
+        <v>2308</v>
       </c>
       <c r="X126" s="7" t="s">
         <v>544</v>
@@ -14787,28 +14784,28 @@
         <v>547</v>
       </c>
       <c r="Q127" s="13" t="s">
-        <v>1963</v>
+        <v>1964</v>
       </c>
       <c r="R127" s="13" t="s">
-        <v>2117</v>
+        <v>2118</v>
       </c>
       <c r="S127" s="13" t="s">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="T127" s="13" t="s">
-        <v>1965</v>
+        <v>1966</v>
       </c>
       <c r="U127" s="13" t="s">
-        <v>2157</v>
+        <v>2158</v>
       </c>
       <c r="V127" s="13" t="s">
-        <v>1966</v>
+        <v>1967</v>
       </c>
       <c r="W127" s="13" t="s">
-        <v>1967</v>
+        <v>1968</v>
       </c>
       <c r="X127" s="13" t="s">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="AG127" s="7" t="s">
         <v>92</v>
@@ -14861,28 +14858,28 @@
         <v>547</v>
       </c>
       <c r="Q128" s="7" t="s">
-        <v>2305</v>
+        <v>2306</v>
       </c>
       <c r="R128" s="7" t="s">
-        <v>2100</v>
+        <v>2101</v>
       </c>
       <c r="S128" s="16" t="s">
-        <v>2198</v>
+        <v>2199</v>
       </c>
       <c r="T128" s="7" t="s">
-        <v>2293</v>
+        <v>2294</v>
       </c>
       <c r="U128" s="7" t="s">
-        <v>2278</v>
+        <v>2279</v>
       </c>
       <c r="V128" s="7" t="s">
-        <v>2175</v>
+        <v>2176</v>
       </c>
       <c r="W128" s="7" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
       <c r="X128" s="7" t="s">
-        <v>2229</v>
+        <v>2230</v>
       </c>
       <c r="Y128" s="7" t="s">
         <v>511</v>
@@ -14932,7 +14929,7 @@
         <v>552</v>
       </c>
       <c r="R129" s="7" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
       <c r="S129" s="7" t="s">
         <v>553</v>
@@ -14982,10 +14979,10 @@
         <v>547</v>
       </c>
       <c r="Q130" s="7" t="s">
-        <v>2313</v>
+        <v>2314</v>
       </c>
       <c r="R130" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S130" s="7" t="s">
         <v>540</v>
@@ -14994,13 +14991,13 @@
         <v>561</v>
       </c>
       <c r="U130" s="7" t="s">
-        <v>2279</v>
+        <v>2280</v>
       </c>
       <c r="V130" s="7" t="s">
         <v>562</v>
       </c>
       <c r="W130" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X130" s="7" t="s">
         <v>563</v>
@@ -15080,28 +15077,28 @@
         <v>566</v>
       </c>
       <c r="Q131" s="13" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="R131" s="13" t="s">
-        <v>1970</v>
+        <v>1971</v>
       </c>
       <c r="S131" s="13" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="T131" s="13" t="s">
-        <v>1972</v>
+        <v>1973</v>
       </c>
       <c r="U131" s="13" t="s">
-        <v>2158</v>
+        <v>2159</v>
       </c>
       <c r="V131" s="13" t="s">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="W131" s="13" t="s">
-        <v>1974</v>
+        <v>1975</v>
       </c>
       <c r="X131" s="13" t="s">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="AG131" s="7" t="s">
         <v>92</v>
@@ -15154,28 +15151,28 @@
         <v>566</v>
       </c>
       <c r="Q132" s="7" t="s">
-        <v>2265</v>
+        <v>2266</v>
       </c>
       <c r="R132" s="7" t="s">
-        <v>2101</v>
+        <v>2102</v>
       </c>
       <c r="S132" s="16" t="s">
-        <v>2199</v>
+        <v>2200</v>
       </c>
       <c r="T132" s="7" t="s">
-        <v>2294</v>
+        <v>2295</v>
       </c>
       <c r="U132" s="7" t="s">
-        <v>2280</v>
+        <v>2281</v>
       </c>
       <c r="V132" s="7" t="s">
-        <v>2176</v>
+        <v>2177</v>
       </c>
       <c r="W132" s="7" t="s">
-        <v>2230</v>
+        <v>2231</v>
       </c>
       <c r="X132" s="7" t="s">
-        <v>2231</v>
+        <v>2232</v>
       </c>
       <c r="Y132" s="7" t="s">
         <v>511</v>
@@ -15225,7 +15222,7 @@
         <v>571</v>
       </c>
       <c r="R133" s="7" t="s">
-        <v>2133</v>
+        <v>2134</v>
       </c>
       <c r="S133" s="7" t="s">
         <v>572</v>
@@ -15275,10 +15272,10 @@
         <v>566</v>
       </c>
       <c r="Q134" s="7" t="s">
-        <v>2314</v>
+        <v>2315</v>
       </c>
       <c r="R134" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S134" s="7" t="s">
         <v>540</v>
@@ -15293,7 +15290,7 @@
         <v>582</v>
       </c>
       <c r="W134" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X134" s="7" t="s">
         <v>583</v>
@@ -15373,28 +15370,28 @@
         <v>586</v>
       </c>
       <c r="Q135" s="13" t="s">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="R135" s="13" t="s">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="S135" s="13" t="s">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="T135" s="13" t="s">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="U135" s="13" t="s">
-        <v>2282</v>
+        <v>2283</v>
       </c>
       <c r="V135" s="13" t="s">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="W135" s="13" t="s">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="X135" s="13" t="s">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="AG135" s="7" t="s">
         <v>92</v>
@@ -15447,28 +15444,28 @@
         <v>586</v>
       </c>
       <c r="Q136" s="7" t="s">
-        <v>2266</v>
+        <v>2267</v>
       </c>
       <c r="R136" s="7" t="s">
-        <v>2102</v>
+        <v>2103</v>
       </c>
       <c r="S136" s="16" t="s">
-        <v>2200</v>
+        <v>2201</v>
       </c>
       <c r="T136" s="7" t="s">
-        <v>2295</v>
+        <v>2296</v>
       </c>
       <c r="U136" s="7" t="s">
-        <v>2281</v>
+        <v>2282</v>
       </c>
       <c r="V136" s="7" t="s">
-        <v>2177</v>
+        <v>2178</v>
       </c>
       <c r="W136" s="7" t="s">
-        <v>2232</v>
+        <v>2233</v>
       </c>
       <c r="X136" s="7" t="s">
-        <v>2233</v>
+        <v>2234</v>
       </c>
       <c r="Y136" s="7" t="s">
         <v>511</v>
@@ -15518,7 +15515,7 @@
         <v>591</v>
       </c>
       <c r="R137" s="7" t="s">
-        <v>2134</v>
+        <v>2135</v>
       </c>
       <c r="S137" s="7" t="s">
         <v>592</v>
@@ -15568,10 +15565,10 @@
         <v>586</v>
       </c>
       <c r="Q138" s="7" t="s">
-        <v>2315</v>
+        <v>2316</v>
       </c>
       <c r="R138" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S138" s="7" t="s">
         <v>540</v>
@@ -15586,7 +15583,7 @@
         <v>602</v>
       </c>
       <c r="W138" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X138" s="7" t="s">
         <v>603</v>
@@ -15666,28 +15663,28 @@
         <v>606</v>
       </c>
       <c r="Q139" s="13" t="s">
-        <v>2270</v>
+        <v>2271</v>
       </c>
       <c r="R139" s="13" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="S139" s="13" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="T139" s="13" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="U139" s="13" t="s">
-        <v>2283</v>
+        <v>2284</v>
       </c>
       <c r="V139" s="13" t="s">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="W139" s="13" t="s">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="X139" s="13" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="AG139" s="7" t="s">
         <v>92</v>
@@ -15740,28 +15737,28 @@
         <v>606</v>
       </c>
       <c r="Q140" s="7" t="s">
-        <v>2269</v>
+        <v>2270</v>
       </c>
       <c r="R140" s="7" t="s">
-        <v>2103</v>
+        <v>2104</v>
       </c>
       <c r="S140" s="16" t="s">
-        <v>2201</v>
+        <v>2202</v>
       </c>
       <c r="T140" s="7" t="s">
-        <v>2108</v>
+        <v>2109</v>
       </c>
       <c r="U140" s="7" t="s">
-        <v>2159</v>
+        <v>2160</v>
       </c>
       <c r="V140" s="7" t="s">
-        <v>2178</v>
+        <v>2179</v>
       </c>
       <c r="W140" s="7" t="s">
-        <v>2234</v>
+        <v>2235</v>
       </c>
       <c r="X140" s="7" t="s">
-        <v>2235</v>
+        <v>2236</v>
       </c>
       <c r="Y140" s="7" t="s">
         <v>511</v>
@@ -15808,10 +15805,10 @@
         <v>606</v>
       </c>
       <c r="Q141" s="7" t="s">
-        <v>2268</v>
+        <v>2269</v>
       </c>
       <c r="R141" s="7" t="s">
-        <v>2135</v>
+        <v>2136</v>
       </c>
       <c r="S141" s="7" t="s">
         <v>611</v>
@@ -15861,10 +15858,10 @@
         <v>606</v>
       </c>
       <c r="Q142" s="7" t="s">
-        <v>2316</v>
+        <v>2317</v>
       </c>
       <c r="R142" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S142" s="7" t="s">
         <v>540</v>
@@ -15879,7 +15876,7 @@
         <v>621</v>
       </c>
       <c r="W142" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X142" s="7" t="s">
         <v>622</v>
@@ -15959,28 +15956,28 @@
         <v>625</v>
       </c>
       <c r="Q143" s="13" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="R143" s="13" t="s">
-        <v>2118</v>
+        <v>2119</v>
       </c>
       <c r="S143" s="13" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="T143" s="13" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="U143" s="13" t="s">
-        <v>2160</v>
+        <v>2161</v>
       </c>
       <c r="V143" s="13" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="W143" s="13" t="s">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="X143" s="13" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="AG143" s="7" t="s">
         <v>92</v>
@@ -16033,28 +16030,28 @@
         <v>625</v>
       </c>
       <c r="Q144" s="7" t="s">
-        <v>2267</v>
+        <v>2268</v>
       </c>
       <c r="R144" s="7" t="s">
-        <v>2119</v>
+        <v>2120</v>
       </c>
       <c r="S144" s="16" t="s">
-        <v>2202</v>
+        <v>2203</v>
       </c>
       <c r="T144" s="7" t="s">
-        <v>2109</v>
+        <v>2110</v>
       </c>
       <c r="U144" s="7" t="s">
-        <v>2284</v>
+        <v>2285</v>
       </c>
       <c r="V144" s="7" t="s">
-        <v>2179</v>
+        <v>2180</v>
       </c>
       <c r="W144" s="7" t="s">
-        <v>2236</v>
+        <v>2237</v>
       </c>
       <c r="X144" s="7" t="s">
-        <v>2237</v>
+        <v>2238</v>
       </c>
       <c r="Y144" s="7" t="s">
         <v>511</v>
@@ -16104,7 +16101,7 @@
         <v>630</v>
       </c>
       <c r="R145" s="7" t="s">
-        <v>2136</v>
+        <v>2137</v>
       </c>
       <c r="S145" s="7" t="s">
         <v>631</v>
@@ -16154,10 +16151,10 @@
         <v>625</v>
       </c>
       <c r="Q146" s="7" t="s">
-        <v>2317</v>
+        <v>2318</v>
       </c>
       <c r="R146" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S146" s="7" t="s">
         <v>540</v>
@@ -16172,7 +16169,7 @@
         <v>641</v>
       </c>
       <c r="W146" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X146" s="7" t="s">
         <v>642</v>
@@ -16252,28 +16249,28 @@
         <v>645</v>
       </c>
       <c r="Q147" s="13" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="R147" s="13" t="s">
-        <v>2120</v>
+        <v>2121</v>
       </c>
       <c r="S147" s="13" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="T147" s="13" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="U147" s="13" t="s">
-        <v>2285</v>
+        <v>2286</v>
       </c>
       <c r="V147" s="13" t="s">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="W147" s="13" t="s">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="X147" s="13" t="s">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="AG147" s="7" t="s">
         <v>92</v>
@@ -16326,28 +16323,28 @@
         <v>645</v>
       </c>
       <c r="Q148" s="7" t="s">
-        <v>2271</v>
+        <v>2272</v>
       </c>
       <c r="R148" s="7" t="s">
-        <v>2121</v>
+        <v>2122</v>
       </c>
       <c r="S148" s="16" t="s">
-        <v>2203</v>
+        <v>2204</v>
       </c>
       <c r="T148" s="7" t="s">
-        <v>2296</v>
+        <v>2297</v>
       </c>
       <c r="U148" s="7" t="s">
-        <v>2286</v>
+        <v>2287</v>
       </c>
       <c r="V148" s="7" t="s">
-        <v>2180</v>
+        <v>2181</v>
       </c>
       <c r="W148" s="7" t="s">
-        <v>2238</v>
+        <v>2239</v>
       </c>
       <c r="X148" s="7" t="s">
-        <v>2239</v>
+        <v>2240</v>
       </c>
       <c r="Y148" s="7" t="s">
         <v>511</v>
@@ -16397,7 +16394,7 @@
         <v>650</v>
       </c>
       <c r="R149" s="7" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
       <c r="S149" s="7" t="s">
         <v>651</v>
@@ -16447,10 +16444,10 @@
         <v>645</v>
       </c>
       <c r="Q150" s="7" t="s">
-        <v>2318</v>
+        <v>2319</v>
       </c>
       <c r="R150" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S150" s="7" t="s">
         <v>540</v>
@@ -16465,7 +16462,7 @@
         <v>661</v>
       </c>
       <c r="W150" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X150" s="7" t="s">
         <v>662</v>
@@ -16545,28 +16542,28 @@
         <v>665</v>
       </c>
       <c r="Q151" s="13" t="s">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="R151" s="13" t="s">
-        <v>2122</v>
+        <v>2123</v>
       </c>
       <c r="S151" s="13" t="s">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="T151" s="13" t="s">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="U151" s="13" t="s">
-        <v>2161</v>
+        <v>2162</v>
       </c>
       <c r="V151" s="13" t="s">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="W151" s="13" t="s">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="X151" s="13" t="s">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="AG151" s="7" t="s">
         <v>92</v>
@@ -16619,28 +16616,28 @@
         <v>665</v>
       </c>
       <c r="Q152" s="7" t="s">
-        <v>2272</v>
+        <v>2273</v>
       </c>
       <c r="R152" s="7" t="s">
-        <v>2123</v>
+        <v>2124</v>
       </c>
       <c r="S152" s="16" t="s">
-        <v>2204</v>
+        <v>2205</v>
       </c>
       <c r="T152" s="7" t="s">
-        <v>2297</v>
+        <v>2298</v>
       </c>
       <c r="U152" s="7" t="s">
-        <v>2162</v>
+        <v>2163</v>
       </c>
       <c r="V152" s="7" t="s">
-        <v>2181</v>
+        <v>2182</v>
       </c>
       <c r="W152" s="7" t="s">
-        <v>2240</v>
+        <v>2241</v>
       </c>
       <c r="X152" s="7" t="s">
-        <v>2241</v>
+        <v>2242</v>
       </c>
       <c r="Y152" s="7" t="s">
         <v>511</v>
@@ -16690,7 +16687,7 @@
         <v>670</v>
       </c>
       <c r="R153" s="7" t="s">
-        <v>2138</v>
+        <v>2139</v>
       </c>
       <c r="S153" s="7" t="s">
         <v>671</v>
@@ -16740,10 +16737,10 @@
         <v>665</v>
       </c>
       <c r="Q154" s="7" t="s">
-        <v>2319</v>
+        <v>2320</v>
       </c>
       <c r="R154" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S154" s="7" t="s">
         <v>540</v>
@@ -16758,7 +16755,7 @@
         <v>681</v>
       </c>
       <c r="W154" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X154" s="7" t="s">
         <v>682</v>
@@ -16838,28 +16835,28 @@
         <v>685</v>
       </c>
       <c r="Q155" s="13" t="s">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="R155" s="13" t="s">
-        <v>2124</v>
+        <v>2125</v>
       </c>
       <c r="S155" s="13" t="s">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="T155" s="13" t="s">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="U155" s="13" t="s">
-        <v>2163</v>
+        <v>2164</v>
       </c>
       <c r="V155" s="13" t="s">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="W155" s="13" t="s">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="X155" s="13" t="s">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="AG155" s="7" t="s">
         <v>92</v>
@@ -16912,28 +16909,28 @@
         <v>685</v>
       </c>
       <c r="Q156" s="7" t="s">
-        <v>2273</v>
+        <v>2274</v>
       </c>
       <c r="R156" s="7" t="s">
-        <v>2104</v>
+        <v>2105</v>
       </c>
       <c r="S156" s="16" t="s">
-        <v>2205</v>
+        <v>2206</v>
       </c>
       <c r="T156" s="7" t="s">
-        <v>2298</v>
+        <v>2299</v>
       </c>
       <c r="U156" s="7" t="s">
-        <v>2287</v>
+        <v>2288</v>
       </c>
       <c r="V156" s="7" t="s">
-        <v>2182</v>
+        <v>2183</v>
       </c>
       <c r="W156" s="7" t="s">
-        <v>2242</v>
+        <v>2243</v>
       </c>
       <c r="X156" s="7" t="s">
-        <v>2243</v>
+        <v>2244</v>
       </c>
       <c r="Y156" s="7" t="s">
         <v>511</v>
@@ -16983,7 +16980,7 @@
         <v>690</v>
       </c>
       <c r="R157" s="7" t="s">
-        <v>2139</v>
+        <v>2140</v>
       </c>
       <c r="S157" s="7" t="s">
         <v>691</v>
@@ -17033,10 +17030,10 @@
         <v>685</v>
       </c>
       <c r="Q158" s="7" t="s">
-        <v>2320</v>
+        <v>2321</v>
       </c>
       <c r="R158" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S158" s="7" t="s">
         <v>540</v>
@@ -17051,7 +17048,7 @@
         <v>701</v>
       </c>
       <c r="W158" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X158" s="7" t="s">
         <v>702</v>
@@ -17131,28 +17128,28 @@
         <v>705</v>
       </c>
       <c r="Q159" s="13" t="s">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="R159" s="13" t="s">
-        <v>2125</v>
+        <v>2126</v>
       </c>
       <c r="S159" s="13" t="s">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="T159" s="13" t="s">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="U159" s="13" t="s">
-        <v>2288</v>
+        <v>2289</v>
       </c>
       <c r="V159" s="13" t="s">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="W159" s="13" t="s">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="X159" s="13" t="s">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="AG159" s="7" t="s">
         <v>92</v>
@@ -17205,28 +17202,28 @@
         <v>705</v>
       </c>
       <c r="Q160" s="7" t="s">
-        <v>2274</v>
+        <v>2275</v>
       </c>
       <c r="R160" s="7" t="s">
-        <v>2105</v>
+        <v>2106</v>
       </c>
       <c r="S160" s="16" t="s">
-        <v>2206</v>
+        <v>2207</v>
       </c>
       <c r="T160" s="7" t="s">
-        <v>2299</v>
+        <v>2300</v>
       </c>
       <c r="U160" s="7" t="s">
-        <v>2289</v>
+        <v>2290</v>
       </c>
       <c r="V160" s="7" t="s">
-        <v>2183</v>
+        <v>2184</v>
       </c>
       <c r="W160" s="7" t="s">
-        <v>2244</v>
+        <v>2245</v>
       </c>
       <c r="X160" s="7" t="s">
-        <v>2245</v>
+        <v>2246</v>
       </c>
       <c r="Y160" s="7" t="s">
         <v>511</v>
@@ -17276,7 +17273,7 @@
         <v>710</v>
       </c>
       <c r="R161" s="7" t="s">
-        <v>2140</v>
+        <v>2141</v>
       </c>
       <c r="S161" s="7" t="s">
         <v>711</v>
@@ -17326,10 +17323,10 @@
         <v>705</v>
       </c>
       <c r="Q162" s="7" t="s">
-        <v>2321</v>
+        <v>2322</v>
       </c>
       <c r="R162" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S162" s="7" t="s">
         <v>540</v>
@@ -17344,7 +17341,7 @@
         <v>721</v>
       </c>
       <c r="W162" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X162" s="7" t="s">
         <v>722</v>
@@ -17424,28 +17421,28 @@
         <v>725</v>
       </c>
       <c r="Q163" s="13" t="s">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="R163" s="13" t="s">
-        <v>2126</v>
+        <v>2127</v>
       </c>
       <c r="S163" s="13" t="s">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="T163" s="13" t="s">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="U163" s="13" t="s">
-        <v>2164</v>
+        <v>2165</v>
       </c>
       <c r="V163" s="13" t="s">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="W163" s="13" t="s">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="X163" s="13" t="s">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="AG163" s="7" t="s">
         <v>92</v>
@@ -17498,28 +17495,28 @@
         <v>725</v>
       </c>
       <c r="Q164" s="7" t="s">
-        <v>2275</v>
+        <v>2276</v>
       </c>
       <c r="R164" s="7" t="s">
-        <v>2127</v>
+        <v>2128</v>
       </c>
       <c r="S164" s="16" t="s">
-        <v>2207</v>
+        <v>2208</v>
       </c>
       <c r="T164" s="7" t="s">
-        <v>2300</v>
+        <v>2301</v>
       </c>
       <c r="U164" s="7" t="s">
-        <v>2165</v>
+        <v>2166</v>
       </c>
       <c r="V164" s="7" t="s">
-        <v>2184</v>
+        <v>2185</v>
       </c>
       <c r="W164" s="7" t="s">
-        <v>2246</v>
+        <v>2247</v>
       </c>
       <c r="X164" s="7" t="s">
-        <v>2247</v>
+        <v>2248</v>
       </c>
       <c r="Y164" s="7" t="s">
         <v>511</v>
@@ -17569,7 +17566,7 @@
         <v>730</v>
       </c>
       <c r="R165" s="7" t="s">
-        <v>2141</v>
+        <v>2142</v>
       </c>
       <c r="S165" s="7" t="s">
         <v>731</v>
@@ -17619,10 +17616,10 @@
         <v>725</v>
       </c>
       <c r="Q166" s="7" t="s">
-        <v>2322</v>
+        <v>2323</v>
       </c>
       <c r="R166" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S166" s="7" t="s">
         <v>540</v>
@@ -17637,7 +17634,7 @@
         <v>741</v>
       </c>
       <c r="W166" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X166" s="7" t="s">
         <v>742</v>
@@ -17717,28 +17714,28 @@
         <v>745</v>
       </c>
       <c r="Q167" s="13" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="R167" s="13" t="s">
-        <v>2128</v>
+        <v>2129</v>
       </c>
       <c r="S167" s="13" t="s">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="T167" s="13" t="s">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="U167" s="13" t="s">
-        <v>2166</v>
+        <v>2167</v>
       </c>
       <c r="V167" s="13" t="s">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="W167" s="13" t="s">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="X167" s="13" t="s">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="AG167" s="7" t="s">
         <v>92</v>
@@ -17791,28 +17788,28 @@
         <v>745</v>
       </c>
       <c r="Q168" s="7" t="s">
-        <v>2276</v>
+        <v>2277</v>
       </c>
       <c r="R168" s="7" t="s">
-        <v>2106</v>
+        <v>2107</v>
       </c>
       <c r="S168" s="16" t="s">
-        <v>2208</v>
+        <v>2209</v>
       </c>
       <c r="T168" s="7" t="s">
-        <v>2301</v>
+        <v>2302</v>
       </c>
       <c r="U168" s="7" t="s">
-        <v>2167</v>
+        <v>2168</v>
       </c>
       <c r="V168" s="7" t="s">
-        <v>2185</v>
+        <v>2186</v>
       </c>
       <c r="W168" s="7" t="s">
-        <v>2248</v>
+        <v>2249</v>
       </c>
       <c r="X168" s="7" t="s">
-        <v>2249</v>
+        <v>2250</v>
       </c>
       <c r="Y168" s="7" t="s">
         <v>511</v>
@@ -17862,7 +17859,7 @@
         <v>750</v>
       </c>
       <c r="R169" s="7" t="s">
-        <v>2142</v>
+        <v>2143</v>
       </c>
       <c r="S169" s="7" t="s">
         <v>751</v>
@@ -17912,10 +17909,10 @@
         <v>745</v>
       </c>
       <c r="Q170" s="7" t="s">
-        <v>2323</v>
+        <v>2324</v>
       </c>
       <c r="R170" s="7" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="S170" s="7" t="s">
         <v>540</v>
@@ -17930,7 +17927,7 @@
         <v>761</v>
       </c>
       <c r="W170" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X170" s="7" t="s">
         <v>762</v>
@@ -18010,28 +18007,28 @@
         <v>765</v>
       </c>
       <c r="Q171" s="13" t="s">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="R171" s="13" t="s">
-        <v>2129</v>
+        <v>2130</v>
       </c>
       <c r="S171" s="13" t="s">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="T171" s="13" t="s">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="U171" s="13" t="s">
-        <v>2168</v>
+        <v>2169</v>
       </c>
       <c r="V171" s="13" t="s">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="W171" s="13" t="s">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="X171" s="13" t="s">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="AG171" s="7" t="s">
         <v>92</v>
@@ -18084,28 +18081,28 @@
         <v>765</v>
       </c>
       <c r="Q172" s="7" t="s">
-        <v>2277</v>
+        <v>2278</v>
       </c>
       <c r="R172" s="7" t="s">
-        <v>2107</v>
+        <v>2108</v>
       </c>
       <c r="S172" s="16" t="s">
-        <v>2209</v>
+        <v>2210</v>
       </c>
       <c r="T172" s="7" t="s">
-        <v>2302</v>
+        <v>2303</v>
       </c>
       <c r="U172" s="7" t="s">
-        <v>2169</v>
+        <v>2170</v>
       </c>
       <c r="V172" s="7" t="s">
-        <v>2186</v>
+        <v>2187</v>
       </c>
       <c r="W172" s="7" t="s">
-        <v>2250</v>
+        <v>2251</v>
       </c>
       <c r="X172" s="7" t="s">
-        <v>2251</v>
+        <v>2252</v>
       </c>
       <c r="Y172" s="7" t="s">
         <v>511</v>
@@ -18155,7 +18152,7 @@
         <v>770</v>
       </c>
       <c r="R173" s="7" t="s">
-        <v>2143</v>
+        <v>2144</v>
       </c>
       <c r="S173" s="7" t="s">
         <v>771</v>
@@ -18205,10 +18202,10 @@
         <v>765</v>
       </c>
       <c r="Q174" s="7" t="s">
-        <v>2324</v>
+        <v>2325</v>
       </c>
       <c r="R174" s="7" t="s">
-        <v>2144</v>
+        <v>2145</v>
       </c>
       <c r="S174" s="7" t="s">
         <v>779</v>
@@ -18223,7 +18220,7 @@
         <v>782</v>
       </c>
       <c r="W174" s="7" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="X174" s="7" t="s">
         <v>783</v>
@@ -18335,7 +18332,7 @@
         <v>793</v>
       </c>
       <c r="V176" s="7" t="s">
-        <v>2308</v>
+        <v>2309</v>
       </c>
       <c r="W176" s="7" t="s">
         <v>794</v>
@@ -18695,28 +18692,28 @@
         <v>827</v>
       </c>
       <c r="Q185" s="7" t="s">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="R185" s="7" t="s">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="S185" s="7" t="s">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="T185" s="7" t="s">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="U185" s="7" t="s">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="V185" s="7" t="s">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="W185" s="7" t="s">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="X185" s="7" t="s">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="Y185" s="7" t="s">
         <v>826</v>
@@ -18763,28 +18760,28 @@
         <v>827</v>
       </c>
       <c r="Q186" s="7" t="s">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="R186" s="7" t="s">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="S186" s="7" t="s">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="T186" s="7" t="s">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="U186" s="7" t="s">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="V186" s="7" t="s">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="W186" s="7" t="s">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="X186" s="7" t="s">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="AO186" s="25"/>
       <c r="AP186" s="25"/>
@@ -18819,16 +18816,16 @@
         <v>873</v>
       </c>
       <c r="R187" s="7" t="s">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="S187" s="7" t="s">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="T187" s="7" t="s">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="U187" s="7" t="s">
-        <v>2056</v>
+        <v>2057</v>
       </c>
       <c r="V187" s="7" t="s">
         <v>873</v>
@@ -18837,7 +18834,7 @@
         <v>873</v>
       </c>
       <c r="X187" s="7" t="s">
-        <v>2057</v>
+        <v>2058</v>
       </c>
       <c r="Y187" s="7" t="s">
         <v>831</v>
@@ -19155,28 +19152,28 @@
         <v>869</v>
       </c>
       <c r="Q193" s="13" t="s">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="R193" s="13" t="s">
-        <v>2058</v>
+        <v>2059</v>
       </c>
       <c r="S193" s="13" t="s">
-        <v>2059</v>
+        <v>2060</v>
       </c>
       <c r="T193" s="13" t="s">
-        <v>2060</v>
+        <v>2061</v>
       </c>
       <c r="U193" s="13" t="s">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="V193" s="13" t="s">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="W193" s="13" t="s">
-        <v>2061</v>
+        <v>2062</v>
       </c>
       <c r="X193" s="13" t="s">
-        <v>2062</v>
+        <v>2063</v>
       </c>
       <c r="Y193" s="7" t="s">
         <v>826</v>
@@ -19223,28 +19220,28 @@
         <v>869</v>
       </c>
       <c r="Q194" s="13" t="s">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="R194" s="13" t="s">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="S194" s="13" t="s">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="T194" s="13" t="s">
-        <v>2063</v>
+        <v>2064</v>
       </c>
       <c r="U194" s="13" t="s">
-        <v>2064</v>
+        <v>2065</v>
       </c>
       <c r="V194" s="13" t="s">
-        <v>2065</v>
+        <v>2066</v>
       </c>
       <c r="W194" s="13" t="s">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="X194" s="13" t="s">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="AO194" s="25"/>
       <c r="AP194" s="25"/>
@@ -19276,16 +19273,16 @@
         <v>873</v>
       </c>
       <c r="R195" s="13" t="s">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="S195" s="13" t="s">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="T195" s="13" t="s">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="U195" s="13" t="s">
-        <v>2056</v>
+        <v>2057</v>
       </c>
       <c r="V195" s="13" t="s">
         <v>873</v>
@@ -19294,7 +19291,7 @@
         <v>873</v>
       </c>
       <c r="X195" s="13" t="s">
-        <v>2057</v>
+        <v>2058</v>
       </c>
       <c r="Y195" s="7" t="s">
         <v>831</v>
@@ -22543,10 +22540,10 @@
   <dimension ref="A1:L174"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -24259,28 +24256,28 @@
         <v>1293</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>2066</v>
+        <v>2067</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>2067</v>
+        <v>2068</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>2068</v>
+        <v>2069</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>2069</v>
+        <v>2070</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>2070</v>
+        <v>2071</v>
       </c>
       <c r="J50" s="15" t="s">
-        <v>2071</v>
+        <v>2072</v>
       </c>
       <c r="K50" s="14" t="s">
-        <v>2072</v>
+        <v>2073</v>
       </c>
       <c r="L50" s="14" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -24294,28 +24291,28 @@
         <v>1295</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>2074</v>
+        <v>2075</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>2075</v>
+        <v>2076</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>2076</v>
+        <v>2077</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>2077</v>
+        <v>2078</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>2078</v>
+        <v>2079</v>
       </c>
       <c r="J51" s="15" t="s">
-        <v>2079</v>
+        <v>2080</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>2080</v>
+        <v>2081</v>
       </c>
       <c r="L51" s="14" t="s">
-        <v>2081</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -25242,7 +25239,7 @@
         <v>1502</v>
       </c>
       <c r="F78" t="s">
-        <v>2145</v>
+        <v>2146</v>
       </c>
       <c r="G78" t="s">
         <v>1502</v>
@@ -25251,7 +25248,7 @@
         <v>1502</v>
       </c>
       <c r="I78" t="s">
-        <v>2170</v>
+        <v>2171</v>
       </c>
       <c r="J78" t="s">
         <v>1502</v>
@@ -25321,7 +25318,7 @@
         <v>1518</v>
       </c>
       <c r="I80" t="s">
-        <v>2290</v>
+        <v>2291</v>
       </c>
       <c r="J80" t="s">
         <v>1519</v>
@@ -25414,28 +25411,28 @@
         <v>1543</v>
       </c>
       <c r="E83" s="14" t="s">
-        <v>2082</v>
+        <v>2083</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>2083</v>
+        <v>2084</v>
       </c>
       <c r="G83" s="14" t="s">
-        <v>2084</v>
+        <v>2085</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>2085</v>
+        <v>2086</v>
       </c>
       <c r="I83" s="14" t="s">
-        <v>2086</v>
+        <v>2087</v>
       </c>
       <c r="J83" s="15" t="s">
-        <v>2087</v>
+        <v>2088</v>
       </c>
       <c r="K83" s="14" t="s">
-        <v>2088</v>
+        <v>2089</v>
       </c>
       <c r="L83" s="14" t="s">
-        <v>2089</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -28704,13 +28701,13 @@
         <v>1872</v>
       </c>
       <c r="B2" t="s">
-        <v>2349</v>
+        <v>2350</v>
       </c>
       <c r="C2" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D2" t="s">
         <v>2351</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2350</v>
       </c>
       <c r="E2" t="str">
         <f>$D2</f>
@@ -28750,13 +28747,13 @@
         <v>1872</v>
       </c>
       <c r="B3" t="s">
+        <v>2353</v>
+      </c>
+      <c r="C3" t="s">
         <v>2352</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>2351</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2350</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:L21" si="1">$D3</f>
@@ -28796,13 +28793,13 @@
         <v>1872</v>
       </c>
       <c r="B4" t="s">
-        <v>2353</v>
+        <v>2354</v>
       </c>
       <c r="C4" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D4" t="s">
         <v>2351</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2350</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
@@ -28842,13 +28839,13 @@
         <v>1872</v>
       </c>
       <c r="B5" t="s">
-        <v>2354</v>
+        <v>2355</v>
       </c>
       <c r="C5" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D5" t="s">
         <v>2351</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2350</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
@@ -28888,13 +28885,13 @@
         <v>1872</v>
       </c>
       <c r="B6" t="s">
-        <v>2355</v>
+        <v>2356</v>
       </c>
       <c r="C6" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D6" t="s">
         <v>2351</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2350</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
@@ -28934,13 +28931,13 @@
         <v>1873</v>
       </c>
       <c r="B7" t="s">
-        <v>2356</v>
+        <v>2357</v>
       </c>
       <c r="C7" t="s">
-        <v>2349</v>
+        <v>2350</v>
       </c>
       <c r="D7" t="s">
-        <v>2357</v>
+        <v>2358</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
@@ -28980,13 +28977,13 @@
         <v>1873</v>
       </c>
       <c r="B8" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2353</v>
+      </c>
+      <c r="D8" t="s">
         <v>2358</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2352</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2357</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
@@ -29026,13 +29023,13 @@
         <v>1873</v>
       </c>
       <c r="B9" t="s">
-        <v>2359</v>
+        <v>2360</v>
       </c>
       <c r="C9" t="s">
-        <v>2353</v>
+        <v>2354</v>
       </c>
       <c r="D9" t="s">
-        <v>2357</v>
+        <v>2358</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
@@ -29072,13 +29069,13 @@
         <v>1873</v>
       </c>
       <c r="B10" t="s">
-        <v>2360</v>
+        <v>2361</v>
       </c>
       <c r="C10" t="s">
-        <v>2354</v>
+        <v>2355</v>
       </c>
       <c r="D10" t="s">
-        <v>2357</v>
+        <v>2358</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
@@ -29118,13 +29115,13 @@
         <v>1873</v>
       </c>
       <c r="B11" t="s">
-        <v>2361</v>
+        <v>2362</v>
       </c>
       <c r="C11" t="s">
-        <v>2355</v>
+        <v>2356</v>
       </c>
       <c r="D11" t="s">
-        <v>2357</v>
+        <v>2358</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
@@ -29164,13 +29161,13 @@
         <v>1874</v>
       </c>
       <c r="B12" t="s">
-        <v>2362</v>
+        <v>2363</v>
       </c>
       <c r="C12" t="s">
-        <v>2356</v>
+        <v>2357</v>
       </c>
       <c r="D12" t="s">
-        <v>2363</v>
+        <v>2364</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
@@ -29210,13 +29207,13 @@
         <v>1874</v>
       </c>
       <c r="B13" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2359</v>
+      </c>
+      <c r="D13" t="s">
         <v>2364</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2358</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2363</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
@@ -29256,13 +29253,13 @@
         <v>1874</v>
       </c>
       <c r="B14" t="s">
-        <v>2365</v>
+        <v>2366</v>
       </c>
       <c r="C14" t="s">
-        <v>2359</v>
+        <v>2360</v>
       </c>
       <c r="D14" t="s">
-        <v>2363</v>
+        <v>2364</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
@@ -29302,13 +29299,13 @@
         <v>1874</v>
       </c>
       <c r="B15" t="s">
-        <v>2366</v>
+        <v>2367</v>
       </c>
       <c r="C15" t="s">
-        <v>2360</v>
+        <v>2361</v>
       </c>
       <c r="D15" t="s">
-        <v>2363</v>
+        <v>2364</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
@@ -29348,13 +29345,13 @@
         <v>1874</v>
       </c>
       <c r="B16" t="s">
-        <v>2367</v>
+        <v>2368</v>
       </c>
       <c r="C16" t="s">
-        <v>2361</v>
+        <v>2362</v>
       </c>
       <c r="D16" t="s">
-        <v>2363</v>
+        <v>2364</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
@@ -29391,232 +29388,232 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>2368</v>
+        <v>1875</v>
       </c>
       <c r="B17" t="s">
         <v>2369</v>
       </c>
       <c r="C17" t="s">
-        <v>2362</v>
+        <v>2363</v>
       </c>
       <c r="D17" t="s">
-        <v>2370</v>
+        <v>85</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>2368</v>
+        <v>1875</v>
       </c>
       <c r="B18" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="C18" t="s">
-        <v>2364</v>
+        <v>2365</v>
       </c>
       <c r="D18" t="s">
-        <v>2370</v>
+        <v>85</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>2368</v>
+        <v>1875</v>
       </c>
       <c r="B19" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="C19" t="s">
-        <v>2365</v>
+        <v>2366</v>
       </c>
       <c r="D19" t="s">
-        <v>2370</v>
+        <v>85</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>2368</v>
+        <v>1875</v>
       </c>
       <c r="B20" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="C20" t="s">
-        <v>2366</v>
+        <v>2367</v>
       </c>
       <c r="D20" t="s">
-        <v>2370</v>
+        <v>85</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2373</v>
+      </c>
+      <c r="C21" t="s">
         <v>2368</v>
       </c>
-      <c r="B21" t="s">
-        <v>2374</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2367</v>
-      </c>
       <c r="D21" t="s">
-        <v>2370</v>
+        <v>85</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="1"/>
-        <v>Level 4 Geography</v>
+        <v>EA</v>
       </c>
     </row>
   </sheetData>
@@ -29645,42 +29642,42 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="B1" t="s">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="C1" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="D1" t="s">
-        <v>1878</v>
+        <v>1879</v>
       </c>
       <c r="E1" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
       <c r="F1" t="s">
-        <v>1880</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>2325</v>
+        <v>2326</v>
       </c>
       <c r="B2" t="s">
-        <v>2328</v>
+        <v>2329</v>
       </c>
       <c r="C2" t="s">
         <v>1854</v>
       </c>
       <c r="D2" t="s">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="E2" t="s">
-        <v>1882</v>
+        <v>1883</v>
       </c>
       <c r="F2" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
     </row>
   </sheetData>
@@ -29716,22 +29713,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>1884</v>
+        <v>1885</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1887</v>
+        <v>1888</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>1888</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -29739,19 +29736,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1889</v>
+        <v>1890</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>1199</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1891</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -29762,16 +29759,16 @@
         <v>42824</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>1199</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>1896</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -29779,16 +29776,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>1892</v>
+        <v>1893</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>1894</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -29799,16 +29796,16 @@
         <v>42829</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>1199</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1897</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -29819,16 +29816,16 @@
         <v>42829</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>1199</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1898</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -29839,16 +29836,16 @@
         <v>42829</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>1899</v>
+        <v>1900</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>1900</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -29859,16 +29856,16 @@
         <v>42829</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1199</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>1902</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -29879,16 +29876,16 @@
         <v>42829</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>1912</v>
+        <v>1913</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>1904</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -29899,16 +29896,16 @@
         <v>42829</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>1913</v>
+        <v>1914</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>1905</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -29919,16 +29916,16 @@
         <v>42829</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>1914</v>
+        <v>1915</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>1906</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -29939,16 +29936,16 @@
         <v>42829</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>1915</v>
+        <v>1916</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>1907</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -29959,16 +29956,16 @@
         <v>42829</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>1916</v>
+        <v>1917</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>1908</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -29979,16 +29976,16 @@
         <v>42829</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>1917</v>
+        <v>1918</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>1909</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -29999,16 +29996,16 @@
         <v>42829</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>1918</v>
+        <v>1919</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>1910</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -30019,16 +30016,16 @@
         <v>42829</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>1911</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -30039,16 +30036,16 @@
         <v>42829</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>1920</v>
+        <v>1921</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>1921</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -30059,16 +30056,16 @@
         <v>42859</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>1929</v>
+        <v>1930</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>2091</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -30079,16 +30076,16 @@
         <v>42890</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>2092</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -30099,16 +30096,16 @@
         <v>42890</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>2092</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -30119,16 +30116,16 @@
         <v>42920</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>2092</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -30139,16 +30136,16 @@
         <v>42920</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>2092</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -30159,16 +30156,16 @@
         <v>42920</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>2310</v>
+        <v>2311</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>2311</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -30179,16 +30176,16 @@
         <v>42951</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>2092</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -30199,16 +30196,16 @@
         <v>43043</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>2310</v>
+        <v>2311</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>2326</v>
+        <v>2327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>